<commit_message>
feat: connect fe and be in btn02
</commit_message>
<xml_diff>
--- a/packages/backend/src/classes/template/gradeboard.xlsx
+++ b/packages/backend/src/classes/template/gradeboard.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -385,37 +385,60 @@
         <v/>
       </c>
       <c r="B1" t="str">
-        <v>GK</v>
+        <v>Cuoi ky</v>
       </c>
       <c r="C1" t="str">
-        <v>CK</v>
+        <v>Giua ky</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Total</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Tran Thanh Hien</v>
+        <v>Nguyen Van A</v>
       </c>
       <c r="B2" t="str">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C2" t="str">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="D2" t="str">
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Tran Thanh Hiennnn</v>
+        <v>Nguyen Van B</v>
       </c>
       <c r="B3" t="str">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="C3" t="str">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="D3" t="str">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Student</v>
+      </c>
+      <c r="B4" t="str">
+        <v>50</v>
+      </c>
+      <c r="C4" t="str">
+        <v>50</v>
+      </c>
+      <c r="D4" t="str">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: request, list and view detail grade review
</commit_message>
<xml_diff>
--- a/packages/backend/src/classes/template/gradeboard.xlsx
+++ b/packages/backend/src/classes/template/gradeboard.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -385,60 +385,55 @@
         <v/>
       </c>
       <c r="B1" t="str">
-        <v>Cuoi ky</v>
+        <v>GK1</v>
       </c>
       <c r="C1" t="str">
-        <v>Giua ky</v>
+        <v>CK1</v>
       </c>
       <c r="D1" t="str">
+        <v>Bonu</v>
+      </c>
+      <c r="E1" t="str">
         <v>Total</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Nguyen Van A</v>
+        <v>Hoa Pham 2</v>
       </c>
       <c r="B2" t="str">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C2" t="str">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D2" t="str">
-        <v>40</v>
+        <v>60</v>
+      </c>
+      <c r="E2" t="str">
+        <v>161</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Nguyen Van B</v>
+        <v>B</v>
       </c>
       <c r="B3" t="str">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C3" t="str">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D3" t="str">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Student</v>
-      </c>
-      <c r="B4" t="str">
-        <v>50</v>
-      </c>
-      <c r="C4" t="str">
-        <v>50</v>
-      </c>
-      <c r="D4" t="str">
-        <v>100</v>
+        <v>300</v>
+      </c>
+      <c r="E3" t="str">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: fix bug in grade structure
</commit_message>
<xml_diff>
--- a/packages/backend/src/classes/template/gradeboard.xlsx
+++ b/packages/backend/src/classes/template/gradeboard.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -385,13 +385,13 @@
         <v/>
       </c>
       <c r="B1" t="str">
-        <v>GK1</v>
+        <v>GK</v>
       </c>
       <c r="C1" t="str">
-        <v>CK1</v>
+        <v>CK</v>
       </c>
       <c r="D1" t="str">
-        <v>Bonu</v>
+        <v>Bonus</v>
       </c>
       <c r="E1" t="str">
         <v>Total</v>
@@ -399,41 +399,58 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Hoa Pham 2</v>
+        <v>Hoa Pham 1</v>
       </c>
       <c r="B2" t="str">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C2" t="str">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D2" t="str">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E2" t="str">
-        <v>161</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>B</v>
+        <v>Hoa Pham 2</v>
       </c>
       <c r="B3" t="str">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C3" t="str">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="D3" t="str">
-        <v>300</v>
+        <v>10</v>
       </c>
       <c r="E3" t="str">
-        <v>362</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Hoa Pham PVH 1</v>
+      </c>
+      <c r="B4" t="str">
+        <v>5</v>
+      </c>
+      <c r="C4" t="str">
+        <v>50</v>
+      </c>
+      <c r="D4" t="str">
+        <v>10</v>
+      </c>
+      <c r="E4" t="str">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>